<commit_message>
finished the backend, starting the frontend
</commit_message>
<xml_diff>
--- a/differences/back/imgtest.xlsx
+++ b/differences/back/imgtest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diuca\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE59699B-DEAA-472B-A269-3BC8D010937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E2D82-D316-4AF4-9FC5-B936F907CEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BB0E2AA0-6AA7-4F59-A272-DF94D0BDC341}"/>
   </bookViews>
@@ -167,7 +167,7 @@
     <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738950/588-2_hhlmgw_tgth0l.png</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738214/588-1_boo31q.png</t>
+    <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738214/588-1_boo31q.pn</t>
   </si>
 </sst>
 </file>
@@ -259,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -283,9 +283,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -608,7 +605,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,13 +631,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="8">
@@ -649,7 +646,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
     </row>

</xml_diff>

<commit_message>
making the front, need to make a canvas overlaping with an image
</commit_message>
<xml_diff>
--- a/differences/back/imgtest.xlsx
+++ b/differences/back/imgtest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diuca\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E2D82-D316-4AF4-9FC5-B936F907CEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2252307-FC94-4898-86F4-76EDCA3E25BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BB0E2AA0-6AA7-4F59-A272-DF94D0BDC341}"/>
   </bookViews>
@@ -167,7 +167,7 @@
     <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738950/588-2_hhlmgw_tgth0l.png</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738214/588-1_boo31q.pn</t>
+    <t>https://res.cloudinary.com/dwbpf1nax/image/upload/v1693738214/588-1_boo31q.png</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="8">
-        <v>45185</v>
+        <v>45192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>